<commit_message>
updating product backlog following sprint 1 demo
</commit_message>
<xml_diff>
--- a/sprints/Product Backlog.xlsx
+++ b/sprints/Product Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan Corley\Dropbox\Work\_teaching\UWG\Capstone\Spring 2022\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lanthorr\git\Capstone\2\sprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3838CCD7-8993-4A1E-AB80-532D3D0EC31E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB48FFF-01F4-4190-BC97-B1E5FCB0405F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="3630" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -591,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,7 +618,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -632,7 +632,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>0</v>
@@ -646,30 +646,30 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>13</v>
+      <c r="A5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -680,10 +680,10 @@
         <v>0</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -694,10 +694,10 @@
         <v>0</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -708,38 +708,38 @@
         <v>0</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>2</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>7</v>
+      <c r="B10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -750,10 +750,10 @@
         <v>0</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -764,10 +764,10 @@
         <v>0</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -778,10 +778,10 @@
         <v>0</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -792,10 +792,10 @@
         <v>0</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -995,8 +995,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D28">
-    <sortCondition ref="A2:A28"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D29">
+    <sortCondition ref="A2:A29"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Product Backlog for Sprint 3
Updated product backlog for sprint 3 to update the required features for the upcoming.
</commit_message>
<xml_diff>
--- a/sprints/Product Backlog.xlsx
+++ b/sprints/Product Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lanthorr\git\Capstone\2\sprints\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aznel\Documents\UWG\2021-2022\spring semester\capstone\CS4982Project\sprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB48FFF-01F4-4190-BC97-B1E5FCB0405F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6EA0D8-195F-4367-8C3A-810C00554E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="3630" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -591,18 +591,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.5703125" customWidth="1"/>
-    <col min="4" max="4" width="192.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.5546875" customWidth="1"/>
+    <col min="4" max="4" width="192.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -616,9 +616,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -630,7 +630,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>0.5</v>
       </c>
@@ -644,7 +644,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>0.5</v>
       </c>
@@ -658,7 +658,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>0.5</v>
       </c>
@@ -672,9 +672,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>0</v>
@@ -686,9 +686,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>0</v>
@@ -700,9 +700,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>0</v>
@@ -714,9 +714,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>0</v>
@@ -728,9 +728,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>0</v>
@@ -742,21 +742,21 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>2</v>
       </c>
@@ -764,13 +764,13 @@
         <v>0</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>2</v>
       </c>
@@ -778,13 +778,13 @@
         <v>0</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>2</v>
       </c>
@@ -792,13 +792,13 @@
         <v>0</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>3</v>
       </c>
@@ -812,7 +812,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>3</v>
       </c>
@@ -826,7 +826,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>4</v>
       </c>
@@ -840,7 +840,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>4</v>
       </c>
@@ -854,7 +854,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>4</v>
       </c>
@@ -868,7 +868,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>5</v>
       </c>
@@ -882,7 +882,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
         <v>6</v>
       </c>
@@ -896,7 +896,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <v>6</v>
       </c>
@@ -910,7 +910,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="7">
         <v>6</v>
       </c>
@@ -924,7 +924,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
         <v>6</v>
       </c>
@@ -938,7 +938,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
         <v>6</v>
       </c>
@@ -952,7 +952,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="8">
         <v>8</v>
       </c>
@@ -966,7 +966,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="9">
         <v>9</v>
       </c>
@@ -980,7 +980,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="10">
         <v>10</v>
       </c>

</xml_diff>